<commit_message>
Added Saftey Overview Document and Updated Publication Data Section with new data
</commit_message>
<xml_diff>
--- a/OpenExo_Publication_Data/Publication_Data/Engineering/Duration_Test_Results.xlsx
+++ b/OpenExo_Publication_Data/Publication_Data/Engineering/Duration_Test_Results.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Biomech_Lab\Jack_W\Exoskeleton_Design_Paper\Exo_Verificiation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Biomech_Lab\Jack_W\OpenExo\Exo_Verificiation\Duration_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9670CC-3E52-4C12-BF6A-68ECF3DADC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBCECFD-677D-480E-B850-8FB37CE44B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F00B01D2-F3B8-4336-80CE-5344C402F9BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F00B01D2-F3B8-4336-80CE-5344C402F9BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hip" sheetId="1" r:id="rId1"/>
-    <sheet name="Ankle" sheetId="2" r:id="rId2"/>
-    <sheet name="Hip&amp;Ankle" sheetId="3" r:id="rId3"/>
+    <sheet name="Hip_Guard" sheetId="5" r:id="rId2"/>
+    <sheet name="Ankle" sheetId="2" r:id="rId3"/>
+    <sheet name="Hip&amp;Ankle" sheetId="3" r:id="rId4"/>
+    <sheet name="Elbow" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
   <si>
     <t xml:space="preserve">Minute </t>
   </si>
@@ -80,6 +82,18 @@
   </si>
   <si>
     <t>Average Ankle Temp [C]</t>
+  </si>
+  <si>
+    <t>Cover Temp [F]</t>
+  </si>
+  <si>
+    <t>Motor Temp [F]</t>
+  </si>
+  <si>
+    <t>Cover Temp [C]</t>
+  </si>
+  <si>
+    <t>Motor Temp [C]</t>
   </si>
 </sst>
 </file>
@@ -155,9 +169,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -195,7 +209,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -301,7 +315,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -443,7 +457,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -453,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE93F6B-7890-4385-A91A-CC1A2CED8B0C}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,11 +1357,368 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E070BB33-82F2-424D-AC83-79F22BDDA3E9}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>70.2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="D2" s="3">
+        <f>(B2-32)*(5/9)</f>
+        <v>21.222222222222225</v>
+      </c>
+      <c r="E2" s="3">
+        <f>(C2-32)*(5/9)</f>
+        <v>21.166666666666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>72.3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D17" si="0">(B3-32)*(5/9)</f>
+        <v>22.388888888888889</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E17" si="1">(C3-32)*(5/9)</f>
+        <v>22.44444444444445</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <f t="shared" ref="A4:A17" si="2">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>76.7</v>
+      </c>
+      <c r="C4" s="2">
+        <v>75.5</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>24.833333333333336</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="1"/>
+        <v>24.166666666666668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="C5" s="2">
+        <v>79.7</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>25.222222222222225</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="1"/>
+        <v>26.500000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>81.8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>86.3</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>27.666666666666668</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>30.166666666666668</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>85.4</v>
+      </c>
+      <c r="C7" s="2">
+        <v>90.2</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>29.666666666666671</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="1"/>
+        <v>32.333333333333336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>85.4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>93.8</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>29.666666666666671</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>34.333333333333336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>88</v>
+      </c>
+      <c r="C9" s="2">
+        <v>93</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>31.111111111111114</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="1"/>
+        <v>33.888888888888893</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>89.3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>99.7</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>31.833333333333332</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="1"/>
+        <v>37.611111111111114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>91.5</v>
+      </c>
+      <c r="C11" s="2">
+        <v>100.6</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>33.055555555555557</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="1"/>
+        <v>38.111111111111107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>93.2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>104.4</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="1"/>
+        <v>40.222222222222229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>94.8</v>
+      </c>
+      <c r="C13" s="2">
+        <v>106.7</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>34.888888888888886</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>96</v>
+      </c>
+      <c r="C14" s="2">
+        <v>109.4</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>35.555555555555557</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>43.000000000000007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>96.8</v>
+      </c>
+      <c r="C15" s="2">
+        <v>112</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>44.444444444444443</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>98.8</v>
+      </c>
+      <c r="C16" s="2">
+        <v>114.1</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>37.111111111111114</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>45.611111111111107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>100.5</v>
+      </c>
+      <c r="C17" s="2">
+        <v>117.2</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>38.055555555555557</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="1"/>
+        <v>47.333333333333336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885672E3-1AFD-4DE7-8589-242519278489}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,7 +2435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5A02CD-4389-427B-B9C2-F4756DED9C16}">
   <dimension ref="A1:J38"/>
   <sheetViews>
@@ -2829,4 +3200,416 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E9E36F7-EBD9-4B73-9A0A-83F5E7423E4B}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="D2" s="2">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(C2,D2)</f>
+        <v>73.25</v>
+      </c>
+      <c r="F2" s="3">
+        <f>(E2-32)*(5/9)</f>
+        <v>22.916666666666668</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <f>A2+2</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>24.9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>75.2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E17" si="0">AVERAGE(C3,D3)</f>
+        <v>75.550000000000011</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F17" si="1">(E3-32)*(5/9)</f>
+        <v>24.194444444444454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <f t="shared" ref="A4:A17" si="2">A3+2</f>
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>24.8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>79.8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>80.2</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="1"/>
+        <v>26.666666666666668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>24.7</v>
+      </c>
+      <c r="C5" s="2">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="D5" s="2">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="1"/>
+        <v>27.222222222222225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>24.7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>83.3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>86.2</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>84.75</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="1"/>
+        <v>29.305555555555557</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>24.6</v>
+      </c>
+      <c r="C7" s="2">
+        <v>84.5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>88.2</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>86.35</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="1"/>
+        <v>30.194444444444443</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>84.6</v>
+      </c>
+      <c r="D8" s="2">
+        <v>90.6</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>87.6</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="1"/>
+        <v>30.888888888888886</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>86</v>
+      </c>
+      <c r="D9" s="2">
+        <v>90.8</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>88.4</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="1"/>
+        <v>31.333333333333339</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="B10" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>83.8</v>
+      </c>
+      <c r="D10" s="2">
+        <v>94.5</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>89.15</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="1"/>
+        <v>31.750000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="B11" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="C11" s="2">
+        <v>86.2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>94.2</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>90.2</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="1"/>
+        <v>32.333333333333336</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B12" s="2">
+        <v>24.3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>93</v>
+      </c>
+      <c r="D12" s="2">
+        <v>94.5</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>93.75</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="1"/>
+        <v>34.305555555555557</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="B13" s="2">
+        <v>24.2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>93.9</v>
+      </c>
+      <c r="D13" s="2">
+        <v>98</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>95.95</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="1"/>
+        <v>35.527777777777779</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2">
+        <v>93.9</v>
+      </c>
+      <c r="D14" s="2">
+        <v>98.7</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>96.300000000000011</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="1"/>
+        <v>35.722222222222229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="B15" s="2">
+        <v>23.9</v>
+      </c>
+      <c r="C15" s="2">
+        <v>93.7</v>
+      </c>
+      <c r="D15" s="2">
+        <v>100</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>96.85</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="1"/>
+        <v>36.027777777777779</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="B16" s="2">
+        <v>23.8</v>
+      </c>
+      <c r="C16" s="2">
+        <v>96.9</v>
+      </c>
+      <c r="D16" s="2">
+        <v>98</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>97.45</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="1"/>
+        <v>36.361111111111114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="B17" s="2">
+        <v>23.8</v>
+      </c>
+      <c r="C17" s="2">
+        <v>97.1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>102.2</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>99.65</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="1"/>
+        <v>37.583333333333336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>